<commit_message>
* updated benchmark and added them to the documentation
</commit_message>
<xml_diff>
--- a/doc/benchmark.xlsx
+++ b/doc/benchmark.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>LocalDb</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Hops</t>
   </si>
   <si>
-    <t>All links to Philosophie with maximum hop count</t>
-  </si>
-  <si>
     <t>All first links to Philosophie</t>
   </si>
   <si>
@@ -54,13 +51,16 @@
   <si>
     <t>&gt; 600</t>
   </si>
+  <si>
+    <t>All links to Jesus with maximum hop count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -100,25 +100,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -134,6 +135,1024 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LocalDb (just count)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.6925388888888883E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7572366666666675E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13384499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20231521111111112</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2207515333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LocalDb (with data)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$15:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.5025288888888888E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8766844444444433E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15111002222222222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23337932222222221</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8813325888888888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neo4j (just count)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$15:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.0433944444444453E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5005600000000016E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.081167777777778E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9856890999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Neo4j (with data)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$15:$W$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.7831911111111109E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14215208888888886</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68187262222222222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8098769444444436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="267989504"/>
+        <c:axId val="267988944"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="267989504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267988944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="267988944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267989504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,72 +1442,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA16"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="27" max="27" width="16.85546875" customWidth="1"/>
+    <col min="2" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Z1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="Z1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="2"/>
+      <c r="AA1" s="9"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="N2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="T2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="T2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
       <c r="Z2" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,766 +1529,786 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="5">
+      <c r="G3" s="6"/>
+      <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>2</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>3</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>4</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>5</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <v>1</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <v>2</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>3</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="4">
         <v>4</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="4">
         <v>5</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="4">
         <v>1</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3" s="4">
         <v>2</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="4">
         <v>3</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3" s="4">
         <v>4</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3" s="4">
         <v>5</v>
       </c>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.38023220000000002</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.44546370000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.49168079999999997</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.59405129999999995</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>2.2790609000000002</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="3">
+      <c r="G4" s="6"/>
+      <c r="H4" s="2">
         <v>0.3215597</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>0.4782788</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>0.51772739999999995</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>0.61648999999999998</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>2.3431093000000001</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>0.45927010000000001</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>0.52511090000000005</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>0.71828610000000004</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>3.9161448000000001</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" s="3">
+      <c r="R4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="2">
         <v>0.40803620000000002</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="2">
         <v>0.67621629999999999</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="2">
         <v>1.6582199</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="2">
         <v>6.6116900000000003</v>
       </c>
-      <c r="X4" s="3"/>
-      <c r="Z4">
+      <c r="X4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="2">
         <v>0.29637570000000002</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="2">
         <v>2.1666672</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>3.7879000000000003E-2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>6.7634E-2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.136186</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.20205390000000001</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>1.9438027</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="3">
+      <c r="G5" s="6"/>
+      <c r="H5" s="2">
         <v>3.5100100000000002E-2</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>6.8387299999999998E-2</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>0.1506439</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>0.23206379999999999</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>1.8803475000000001</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>4.08788E-2</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>7.10533E-2</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>8.8655999999999999E-2</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <v>1.9686844999999999</v>
       </c>
-      <c r="R5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T5" s="3">
+      <c r="R5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="2">
         <v>3.7581799999999999E-2</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5" s="2">
         <v>0.1785399</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="2">
         <v>0.70188269999999997</v>
       </c>
-      <c r="W5" s="3">
+      <c r="W5" s="2">
         <v>4.9433860000000003</v>
       </c>
-      <c r="X5" s="3"/>
-      <c r="Z5">
+      <c r="X5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="2">
         <v>3.2791599999999997E-2</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="2">
         <v>7.5400900000000007E-2</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>3.7484900000000002E-2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>6.6624500000000003E-2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.1339678</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.2004659</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>1.9703295999999999</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="3">
+      <c r="G6" s="6"/>
+      <c r="H6" s="2">
         <v>3.5485599999999999E-2</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>6.8843000000000001E-2</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>0.1498294</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>0.22607849999999999</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>1.9092765</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>3.8760900000000001E-2</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="2">
         <v>7.0898600000000006E-2</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <v>8.8457300000000003E-2</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="2">
         <v>2.8699029999999999</v>
       </c>
-      <c r="R6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" s="3">
+      <c r="R6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="2">
         <v>3.9203799999999997E-2</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="2">
         <v>0.16807</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="2">
         <v>0.7084743</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="2">
         <v>4.6969118999999999</v>
       </c>
-      <c r="X6" s="3"/>
-      <c r="Z6">
+      <c r="X6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="2">
         <v>3.2337600000000001E-2</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="2">
         <v>6.8232500000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>3.6089099999999999E-2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>6.7751000000000006E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.1350779</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.20480119999999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>1.9921525</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="3">
+      <c r="G7" s="6"/>
+      <c r="H7" s="2">
         <v>3.54195E-2</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>7.0252400000000007E-2</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>0.14942620000000001</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>0.22589999999999999</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>1.8735189999999999</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>3.8741600000000001E-2</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="2">
         <v>6.5672800000000003E-2</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <v>8.8902300000000004E-2</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="2">
         <v>1.8543046000000001</v>
       </c>
-      <c r="R7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="R7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="2">
         <v>3.8311699999999997E-2</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="2">
         <v>0.153305</v>
       </c>
-      <c r="V7" s="3">
+      <c r="V7" s="2">
         <v>0.69833690000000004</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="2">
         <v>5.1002225000000001</v>
       </c>
-      <c r="X7" s="3"/>
-      <c r="Z7">
+      <c r="X7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="2">
         <v>3.1851499999999998E-2</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="2">
         <v>4.8005399999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>3.6415099999999999E-2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>6.8960400000000005E-2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.1337449</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0.19801750000000001</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>3.8634702999999999</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="3">
+      <c r="G8" s="6"/>
+      <c r="H8" s="2">
         <v>3.4722799999999998E-2</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>6.8465300000000007E-2</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>0.1509625</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>0.23406920000000001</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>1.9020629</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>3.8352400000000002E-2</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <v>5.4907299999999999E-2</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="2">
         <v>0.1053977</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <v>1.8612419</v>
       </c>
-      <c r="R8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T8" s="3">
+      <c r="R8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="2">
         <v>3.9634500000000003E-2</v>
       </c>
-      <c r="U8" s="3">
+      <c r="U8" s="2">
         <v>0.1436877</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="2">
         <v>0.64734069999999999</v>
       </c>
-      <c r="W8" s="3">
+      <c r="W8" s="2">
         <v>5.6300331999999997</v>
       </c>
-      <c r="X8" s="3"/>
-      <c r="Z8">
+      <c r="X8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="2">
         <v>3.2083500000000001E-2</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="2">
         <v>4.5612699999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3.6129700000000001E-2</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>6.6388799999999998E-2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.13398180000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.20214750000000001</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>2.0287137999999998</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="3">
+      <c r="G9" s="6"/>
+      <c r="H9" s="2">
         <v>3.4674799999999999E-2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>6.8349999999999994E-2</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>0.1494086</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>0.2373741</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>1.8814712</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>3.8622900000000002E-2</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>4.9144599999999997E-2</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>8.7601299999999993E-2</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>1.8995069</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T9" s="3">
+      <c r="R9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="2">
         <v>3.7164299999999997E-2</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9" s="2">
         <v>0.1452831</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="2">
         <v>0.65420979999999995</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9" s="2">
         <v>5.6589146000000001</v>
       </c>
-      <c r="X9" s="3"/>
-      <c r="Z9">
+      <c r="X9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z9" s="2">
         <v>3.2416800000000003E-2</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="2">
         <v>5.0448100000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>3.6394099999999999E-2</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>6.8241599999999999E-2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.13230929999999999</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.20250009999999999</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>1.9315555</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="3">
+      <c r="G10" s="6"/>
+      <c r="H10" s="2">
         <v>3.4616500000000001E-2</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>6.7937399999999995E-2</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>0.1540977</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>0.23786959999999999</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>1.912865</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="2">
         <v>3.91361E-2</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="2">
         <v>5.18968E-2</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <v>8.7790999999999994E-2</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10" s="2">
         <v>1.7627827</v>
       </c>
-      <c r="R10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T10" s="3">
+      <c r="R10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="2">
         <v>4.9928699999999999E-2</v>
       </c>
-      <c r="U10" s="3">
+      <c r="U10" s="2">
         <v>0.138464</v>
       </c>
-      <c r="V10" s="3">
+      <c r="V10" s="2">
         <v>0.690689</v>
       </c>
-      <c r="W10" s="3">
+      <c r="W10" s="2">
         <v>4.1507958</v>
       </c>
-      <c r="X10" s="3"/>
-      <c r="Z10">
+      <c r="X10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z10" s="2">
         <v>3.2154099999999998E-2</v>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="2">
         <v>3.9170200000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>3.6845299999999997E-2</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>6.7722699999999997E-2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.13397110000000001</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>0.20518549999999999</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>1.9983397000000001</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="3">
+      <c r="G11" s="6"/>
+      <c r="H11" s="2">
         <v>3.4765499999999998E-2</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>6.8156599999999998E-2</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>0.1526333</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>0.22808610000000001</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>1.8527171</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>3.9329900000000001E-2</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="2">
         <v>4.9939400000000002E-2</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <v>8.7047100000000002E-2</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11" s="2">
         <v>1.92456</v>
       </c>
-      <c r="R11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T11" s="3">
+      <c r="R11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T11" s="2">
         <v>3.1615499999999998E-2</v>
       </c>
-      <c r="U11" s="3">
+      <c r="U11" s="2">
         <v>0.12834509999999999</v>
       </c>
-      <c r="V11" s="3">
+      <c r="V11" s="2">
         <v>0.66591920000000004</v>
       </c>
-      <c r="W11" s="3">
+      <c r="W11" s="2">
         <v>4.3819378999999996</v>
       </c>
-      <c r="X11" s="3"/>
-      <c r="Z11">
+      <c r="X11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z11" s="2">
         <v>3.1915600000000002E-2</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="2">
         <v>3.8205799999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>3.7830999999999997E-2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>6.72518E-2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>0.13312299999999999</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>0.204536</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>2.1271537</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="3">
+      <c r="G12" s="6"/>
+      <c r="H12" s="2">
         <v>3.5366500000000002E-2</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>6.9589399999999996E-2</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>0.15063360000000001</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="8">
         <v>0.22998479999999999</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>1.8722924000000001</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="2">
         <v>3.8919700000000002E-2</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="2">
         <v>4.1636699999999999E-2</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <v>9.5325999999999994E-2</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="2">
         <v>1.8270679000000001</v>
       </c>
-      <c r="R12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T12" s="3">
+      <c r="R12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="2">
         <v>3.3193599999999997E-2</v>
       </c>
-      <c r="U12" s="3">
+      <c r="U12" s="2">
         <v>0.1056822</v>
       </c>
-      <c r="V12" s="3">
+      <c r="V12" s="2">
         <v>0.66035880000000002</v>
       </c>
-      <c r="W12" s="3">
+      <c r="W12" s="2">
         <v>4.1087226000000001</v>
       </c>
-      <c r="X12" s="3"/>
-      <c r="Z12">
+      <c r="X12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z12" s="2">
         <v>3.2248499999999999E-2</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="2">
         <v>3.8169300000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>3.7260300000000003E-2</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>6.7576499999999998E-2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>0.13224320000000001</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>0.20112930000000001</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>2.131246</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="6">
+      <c r="G13" s="6"/>
+      <c r="H13" s="5">
         <v>3.5076299999999998E-2</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>6.8920200000000001E-2</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>0.15235499999999999</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>0.24898780000000001</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>1.8474417000000001</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <v>5.1163199999999999E-2</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <v>3.9900900000000003E-2</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="5">
         <v>8.8126399999999994E-2</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="5">
         <v>1.9031503999999999</v>
       </c>
-      <c r="R13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T13" s="6">
+      <c r="R13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="5">
         <v>3.3853300000000003E-2</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="5">
         <v>0.11799179999999999</v>
       </c>
-      <c r="V13" s="6">
+      <c r="V13" s="5">
         <v>0.7096422</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13" s="5">
         <v>4.6179680000000003</v>
       </c>
-      <c r="X13" s="6"/>
+      <c r="X13" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="Z13" s="5">
         <v>3.1964800000000002E-2</v>
       </c>
@@ -1265,219 +2317,218 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <f>AVERAGE(B5:B13)</f>
         <v>3.6925388888888883E-2</v>
       </c>
-      <c r="C15" s="3">
-        <f t="shared" ref="C15:L15" si="0">AVERAGE(C5:C13)</f>
+      <c r="C15" s="2">
+        <f t="shared" ref="C15:F15" si="0">AVERAGE(C5:C13)</f>
         <v>6.7572366666666675E-2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>0.13384499999999999</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>0.20231521111111112</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>2.2207515333333334</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
         <f t="shared" ref="H15:L15" si="1">AVERAGE(H5:H13)</f>
         <v>3.5025288888888888E-2</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <f t="shared" si="1"/>
         <v>6.8766844444444433E-2</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <f t="shared" si="1"/>
         <v>0.15111002222222222</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="2">
         <f>AVERAGE(K5:K13)</f>
         <v>0.23337932222222221</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <f t="shared" si="1"/>
         <v>1.8813325888888888</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="2">
         <f>AVERAGE(N5:N13)</f>
         <v>4.0433944444444453E-2</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="2">
         <f>AVERAGE(O5:O13)</f>
         <v>5.5005600000000016E-2</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="2">
         <f>AVERAGE(P5:P13)</f>
         <v>9.081167777777778E-2</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="2">
         <f>AVERAGE(Q5:Q13)</f>
         <v>1.9856890999999999</v>
       </c>
-      <c r="R15" s="3"/>
-      <c r="T15" s="3">
+      <c r="R15" s="2"/>
+      <c r="T15" s="2">
         <f>AVERAGE(T5:T13)</f>
         <v>3.7831911111111109E-2</v>
       </c>
-      <c r="U15" s="3">
+      <c r="U15" s="2">
         <f>AVERAGE(U5:U13)</f>
         <v>0.14215208888888886</v>
       </c>
-      <c r="V15" s="3">
+      <c r="V15" s="2">
         <f>AVERAGE(V5:V13)</f>
         <v>0.68187262222222222</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W15" s="2">
         <f>AVERAGE(W5:W13)</f>
         <v>4.8098769444444436</v>
       </c>
-      <c r="X15" s="3" t="e">
-        <f>AVERAGE(X5:X13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z15" s="3">
+      <c r="X15" s="2"/>
+      <c r="Z15" s="2">
         <f t="shared" ref="Z15:AA15" si="2">AVERAGE(Z5:Z13)</f>
         <v>3.2196000000000002E-2</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="AA15" s="2">
         <f t="shared" si="2"/>
         <v>5.0018077777777788E-2</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <f>_xlfn.STDEV.S(B5:B13)</f>
         <v>7.1030808006886136E-4</v>
       </c>
-      <c r="C16" s="3">
-        <f t="shared" ref="C16:L16" si="3">_xlfn.STDEV.S(C5:C13)</f>
+      <c r="C16" s="2">
+        <f t="shared" ref="C16:F16" si="3">_xlfn.STDEV.S(C5:C13)</f>
         <v>7.7740592517680344E-4</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <f t="shared" si="3"/>
         <v>1.2502729921901076E-3</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="3"/>
         <v>2.3124082227433539E-3</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f t="shared" si="3"/>
         <v>0.62017597508762456</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2">
         <f t="shared" ref="H16:L16" si="4">_xlfn.STDEV.S(H5:H13)</f>
         <v>3.4293825772449392E-4</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <f t="shared" si="4"/>
         <v>7.4009368006880123E-4</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <f t="shared" si="4"/>
         <v>1.6059523014225667E-3</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="2">
         <f>_xlfn.STDEV.S(K5:K13)</f>
         <v>7.3377040112656841E-3</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="2">
         <f t="shared" si="4"/>
         <v>2.3227425253051857E-2</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="2">
         <f>_xlfn.STDEV.S(N5:N13)</f>
         <v>4.0894206267853847E-3</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="2">
         <f>_xlfn.STDEV.S(O5:O13)</f>
         <v>1.1728580120798865E-2</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="2">
         <f>_xlfn.STDEV.S(P5:P13)</f>
         <v>5.9977151544937874E-3</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="2">
         <f>_xlfn.STDEV.S(Q5:Q13)</f>
         <v>0.33684141177900923</v>
       </c>
-      <c r="R16" s="3"/>
-      <c r="T16" s="3">
+      <c r="R16" s="2"/>
+      <c r="T16" s="2">
         <f>_xlfn.STDEV.S(T5:T13)</f>
         <v>5.3407537884282881E-3</v>
       </c>
-      <c r="U16" s="3">
+      <c r="U16" s="2">
         <f>_xlfn.STDEV.S(U5:U13)</f>
         <v>2.3049856205432463E-2</v>
       </c>
-      <c r="V16" s="3">
+      <c r="V16" s="2">
         <f>_xlfn.STDEV.S(V5:V13)</f>
         <v>2.4756424660973251E-2</v>
       </c>
-      <c r="W16" s="3">
+      <c r="W16" s="2">
         <f>_xlfn.STDEV.S(W5:W13)</f>
         <v>0.57601798727384146</v>
       </c>
-      <c r="X16" s="3" t="e">
-        <f>_xlfn.STDEV.S(X5:X13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z16" s="3">
+      <c r="X16" s="2"/>
+      <c r="Z16" s="2">
         <f t="shared" ref="Z16:AA16" si="5">_xlfn.STDEV.S(Z5:Z13)</f>
         <v>2.939958588143712E-4</v>
       </c>
-      <c r="AA16" s="3">
+      <c r="AA16" s="2">
         <f t="shared" si="5"/>
         <v>1.3261351745182077E-2</v>
       </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="N2:R2"/>
-    <mergeCell ref="B1:L1"/>
     <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="T2:X2"/>
+    <mergeCell ref="B1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>